<commit_message>
Added better validation for fund units
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_unit_setting.xlsx
+++ b/public/sample_uploads/fund_unit_setting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Desktop\bulk files with notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA29307-1602-4220-8199-F60BABC847CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D30C76-B048-481F-9609-DC3027739CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,16 +236,16 @@
     <t>SAAS Fund</t>
   </si>
   <si>
-    <t>Serie A</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Serie B</t>
-  </si>
-  <si>
     <t>Fund*</t>
+  </si>
+  <si>
+    <t>Series A</t>
+  </si>
+  <si>
+    <t>Series B</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -668,7 +668,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -692,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -712,7 +712,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added better tests for FUS import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_unit_setting.xlsx
+++ b/public/sample_uploads/fund_unit_setting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D30C76-B048-481F-9609-DC3027739CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA966EE-D6D4-4DD0-8629-1185E4D3F7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -216,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Class/Series *</t>
   </si>
@@ -246,13 +243,16 @@
   </si>
   <si>
     <t>Series B</t>
+  </si>
+  <si>
+    <t>Carry% (&gt;4x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -298,6 +298,11 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -325,19 +330,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8F4751C8-B9F1-45A2-9D9D-2409C46882F6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -652,7 +657,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -666,7 +671,7 @@
     <col min="7" max="16384" width="8.53125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -685,9 +690,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -706,8 +713,11 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G2" s="3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -725,6 +735,9 @@
       </c>
       <c r="F3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated fund unit setting upload to include gp units (#744)
* Updated fund unit setting upload to include gp units

* Fix case issue in gp units upload
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_unit_setting.xlsx
+++ b/public/sample_uploads/fund_unit_setting.xlsx
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,16 +167,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -198,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">Fund*</t>
   </si>
@@ -215,15 +212,15 @@
     <t xml:space="preserve">Carry %*</t>
   </si>
   <si>
+    <t xml:space="preserve">Gp Units</t>
+  </si>
+  <si>
     <t xml:space="preserve">Update Only</t>
   </si>
   <si>
     <t xml:space="preserve">Isin</t>
   </si>
   <si>
-    <t xml:space="preserve">Carry% (&gt;4x)</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAAS Fund</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t xml:space="preserve">Series B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">INE0J1Y01018</t>
@@ -249,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -293,13 +293,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -309,14 +302,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -380,24 +365,20 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,7 +575,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -604,11 +585,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="1" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,13 +610,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -655,12 +638,12 @@
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I2" s="0"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -679,19 +662,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I3" s="0"/>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F1003" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:G1003" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>